<commit_message>
Today, the estimated hash rate per second
269 explanations on 132 pages. Today the estimated hash rate per second.
</commit_message>
<xml_diff>
--- a/MathDIY-datasets.xlsx
+++ b/MathDIY-datasets.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1084">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1089">
   <si>
     <t>MathDIY</t>
   </si>
@@ -44127,6 +44127,78 @@
   <si>
     <t>［subtitle］［description］
 Source: Wikipedia, the free encyclopedia; https://en.wikipedia.org/wiki/Public-benefit_corporation; Recommended: zevia.com; Example/delimination given: Jens T. Hinrichs #MathDIY; latest update: Wednesday, July 28, Year 21 after Y2K, 6:05 pm</t>
+  </si>
+  <si>
+    <t>IY001</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">H = 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> D / T</t>
+    </r>
+  </si>
+  <si>
+    <t>Estimated hash rate (H) per second. A determinant of Yours (Y) in the Internet without Frontiers (IwF).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Methodology: The hashing power is estimated from the number of blocks being mined in the last 24h and the current block difficulty. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">More specifically, given the average time T between mined blocks and a difficulty D, the estimated hash rate per second H is given by the formula H = 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> D / T</t>
+    </r>
+  </si>
+  <si>
+    <t>Source: Blockchain.com; latest update: Tuesday, Nov 16, Year 21 after Y2K, 4:54 pm</t>
   </si>
 </sst>
 </file>
@@ -45478,7 +45550,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F269"/>
+  <dimension ref="A1:F270"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -50872,6 +50944,26 @@
         <v>1083</v>
       </c>
       <c r="F269" t="s" s="10">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="270" ht="86.7" customHeight="1">
+      <c r="A270" t="s" s="9">
+        <v>1084</v>
+      </c>
+      <c r="B270" t="s" s="10">
+        <v>1085</v>
+      </c>
+      <c r="C270" t="s" s="10">
+        <v>1086</v>
+      </c>
+      <c r="D270" t="s" s="10">
+        <v>1087</v>
+      </c>
+      <c r="E270" t="s" s="10">
+        <v>1088</v>
+      </c>
+      <c r="F270" t="s" s="10">
         <v>857</v>
       </c>
     </row>

</xml_diff>

<commit_message>
R051 – R053 Consumer Price Index (.recapitulation)
See how the CPI calculated, updated, weighted and harmonized.
</commit_message>
<xml_diff>
--- a/MathDIY-datasets.xlsx
+++ b/MathDIY-datasets.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1104">
   <si>
     <t>MathDIY</t>
   </si>
@@ -44199,6 +44199,429 @@
   </si>
   <si>
     <t>Source: Blockchain.com; latest update: Tuesday, Nov 16, Year 21 after Y2K, 4:54 pm</t>
+  </si>
+  <si>
+    <t>R051</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>CPI</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> ÷ CPI</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> = p</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> ÷ p</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>Calculating the CPI for a single item</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">          market basket of desired JJJJ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">CPI = —————————————— x 100
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">          market basket of base JJJJ 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">           p</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> of item, given period (updated cost)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">CPI = ———————————————— x 100
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">           p</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> of item, initial period (base cost
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Excerpt retrieved from:
+en.wikipedia.org; 
+title id 1062042105, Consumer Price Index 
+This source was last edited on 25 Dec 2021, at 21:28 (UTC). 
+Source above is available under the 
+Creative Commons Attribution-ShareAlike License; additional terms may apply. By using this source, you agree to the Terms of Use and Privacy Policy. Wikipedia® is a registered trademark of the Wikimedia Foundation, Inc., a non-profit organization. </t>
+  </si>
+  <si>
+    <t>R052</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">             </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">           ∑</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">CPI x weight
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">             </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>i=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">CPI = —————————         
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">             </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">           ∑</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> x weight
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">             </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>i=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Calculating the CPI for multiple items</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">         
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Many but not all price indices are weighted averages using weights that sum to 1 or 100. Also the terms do not necessarily sum to 1 or 100.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Many but not all price indices are weighted averages using weights that sum to 1 or 100. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Example: The prices of 85,000 items from 22,000 stores, and 35,000 rental units are added together and averaged. They are weighted this way: housing 41.4%; food and beverages 17.4%; transport 17.0%; medical care 6.9%; apparel 6.0%; entertainment 4.4%; other 6.9%. Taxes (43%) are not included in CPI computation.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Excerpt retrieved from:
+en.wikipedia.org; 
+title id 1062042105, Consumer Price Index 
+This source was last edited on 25 Dec 2021, at 21:28 (UTC). 
+Source above is available under the 
+Creative Commons Attribution-ShareAlike License; additional terms may apply. By using this source, you agree to the Terms of Use and Privacy Policy. Wikipedia® is a registered trademark of the Wikimedia Foundation, Inc., a non-profit organization. 
+</t>
+  </si>
+  <si>
+    <t>R053</t>
+  </si>
+  <si>
+    <t>HCPI</t>
+  </si>
+  <si>
+    <t>Harmonized Index of Consumer Prices (HICP)</t>
+  </si>
+  <si>
+    <t>By convention, weights are fractions or ratios summing to one, as percentages summing to 100 or as per mille numbers summing to 1000. 
+On the European Union's Harmonized Index of Consumer Prices (HICP), for example, each country computes some 80 prescribed sub-indices, their weighted average constituting the national HICP. The weights for these sub-indices will consist of the sum of the weights of a number of component lower level indices. The classification is according to use, developed in a national accounting context. This is not necessarily the kind of classification that is most appropriate for a consumer price index.</t>
+  </si>
+  <si>
+    <t>Excerpt retrieved from:
+en.wikipedia.org; 
+title id 1062042105, Consumer Price Index 
+This source was last edited on 25 Dec 2021, at 21:28 (UTC). 
+Source above is available under the 
+Creative Commons Attribution-ShareAlike License; additional terms may apply. By using this source, you agree to the Terms of Use and Privacy Policy. Wikipedia® is a registered trademark of the Wikimedia Foundation, Inc., a non-profit organization.</t>
   </si>
 </sst>
 </file>
@@ -45550,7 +45973,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F270"/>
+  <dimension ref="A1:F273"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -46167,7 +46590,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" ht="1325.35" customHeight="1">
+    <row r="31" ht="1115.7" customHeight="1">
       <c r="A31" t="s" s="9">
         <v>132</v>
       </c>
@@ -46187,7 +46610,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" ht="751.6" customHeight="1">
+    <row r="32" ht="634.2" customHeight="1">
       <c r="A32" t="s" s="9">
         <v>137</v>
       </c>
@@ -50965,6 +51388,66 @@
       </c>
       <c r="F270" t="s" s="10">
         <v>857</v>
+      </c>
+    </row>
+    <row r="271" ht="146.7" customHeight="1">
+      <c r="A271" t="s" s="9">
+        <v>1089</v>
+      </c>
+      <c r="B271" t="s" s="10">
+        <v>1090</v>
+      </c>
+      <c r="C271" t="s" s="10">
+        <v>1091</v>
+      </c>
+      <c r="D271" t="s" s="10">
+        <v>1092</v>
+      </c>
+      <c r="E271" t="s" s="10">
+        <v>1093</v>
+      </c>
+      <c r="F271" t="s" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="272" ht="158.7" customHeight="1">
+      <c r="A272" t="s" s="9">
+        <v>1094</v>
+      </c>
+      <c r="B272" t="s" s="10">
+        <v>1095</v>
+      </c>
+      <c r="C272" t="s" s="10">
+        <v>1096</v>
+      </c>
+      <c r="D272" t="s" s="10">
+        <v>1097</v>
+      </c>
+      <c r="E272" t="s" s="10">
+        <v>1098</v>
+      </c>
+      <c r="F272" t="s" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="273" ht="170.7" customHeight="1">
+      <c r="A273" t="s" s="9">
+        <v>1099</v>
+      </c>
+      <c r="B273" t="s" s="10">
+        <v>1100</v>
+      </c>
+      <c r="C273" t="s" s="10">
+        <v>1101</v>
+      </c>
+      <c r="D273" t="s" s="10">
+        <v>1102</v>
+      </c>
+      <c r="E273" t="s" s="10">
+        <v>1103</v>
+      </c>
+      <c r="F273" t="s" s="10">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>